<commit_message>
Added Greece and Romania mapping files and reformatted Turkey file
</commit_message>
<xml_diff>
--- a/res_mapping_schemes/mapping_Turkey_RES.xlsx
+++ b/res_mapping_schemes/mapping_Turkey_RES.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0AF0DB-AD39-1248-95D5-3B247DEDC109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCD1136-BC55-3F49-9080-F4B86CD241E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2560" yWindow="460" windowWidth="25720" windowHeight="14440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_urban" sheetId="1" r:id="rId1"/>
     <sheet name="mapping_rural" sheetId="4" r:id="rId2"/>
-    <sheet name="mapping_Istanbul" sheetId="2" r:id="rId3"/>
+    <sheet name="mapping_istanbul" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="52">
   <si>
     <t>Steel sheet/frame</t>
   </si>
@@ -65,92 +65,6 @@
   </si>
   <si>
     <t>ADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% S/LFM+CDL/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">30% CR/LFINF+CDL/HBET:1-3 
-45% CR/LFINF+CDL/HBET:4-6 
-15% CR/LFINF+CDL/HBET:7- 
-10% CR/LFINF+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">92% CR/LFINF(CBH)+CDL/HBET:1-3 
-5% CR/LFINF(CBH)+CDL/HBET:4-6 
-3% CR/LFINF(CBH)+CDL/HBET:7- </t>
-  </si>
-  <si>
-    <t xml:space="preserve">16% CR/LFINF(CL)+CDL/HBET:1-3 
-44% CR/LFINF(CL)+CDL/HBET:4-6 
-10% CR/LFINF(CL)+CDL/HBET:7- 
-30% MUR+CL/LWAL+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">80% W/LFM+CDN/HBET:1-3 
-20% W/LFM+CDL/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% MUR+STRUB/LWAL+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">50% MUR+CBH/LWAL+CDN/HBET:1-3 
-50% CR/LWAL+CDL/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">35% CR/LWAL+CDL/HBET:1-3 
-10% CR/LWAL+CDL/HBET:4-6 
-55% MUR+CL/LWAL+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">80% W/LWAL+CDN/HBET:1-3 
-20% W/LWAL+CDL/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">45% CR/LDUAL+CDL/HBET:1-3 
-20% CR/LDUAL+CDL/HBET:4-6 
-35% CR/LDUAL+CDL/HBET:7- </t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% CR+PC/LWAL+CDL/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% MUR+CL/LWAL+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% MUR+ADO/LWAL+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20% CR/LDUAL+CDH/HBET:1-3 
-20% CR/LDUAL+CDH/HBET:4-6 
-7% CR/LDUAL+CDH/HBET:7- 
-25% CR/LWAL+CDH/HBET:1-3 
-20% CR/LWAL+CDH/HBET:4-6 
-8% CR/LWAL+CDH/HBET:7- </t>
-  </si>
-  <si>
-    <t xml:space="preserve">92% CR/LFINF(CBH)+CDL/HBET:1-3 
-5% CR/LFINF(CBH)+CDL/HBET:4-6/SOS 
-3% CR/LFINF(CBH)+CDL/HBET:7-/SOS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">23% CR/LFINF(CL)+CDL/HBET:1-3 
-44% CR/LFINF(CL)+CDL/HBET:4-6 
-10% CR/LFINF(CL)+CDL/HBET:7- 
-23% MUR+CL/LWAL+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">95% MUR+STRUB/LWAL+CDN/HBET:1-3 
-5% MUR+STRUB/LWAL+CDN/HBET:4-6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">45% CR/LWAL+CDL/HBET:1-3 
-10% CR/LWAL+CDL/HBET:4-6 
-45% MUR+CL/LWAL+CDN/HBET:1-3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">30% MUR+CBH/LWAL+CDN/HBET:1-3 
-70% CR/LWAL+CDL/HBET:1-3 </t>
   </si>
   <si>
     <t xml:space="preserve">RES_2017
@@ -300,6 +214,50 @@
   <si>
     <t>25% CR/LDUAL+CDH/HBET:1-3
 15% CR/LDUAL+CDH/HBET:4-6
+7% CR/LDUAL+CDH/HBET:7-
+25% CR/LWAL+CDH/HBET:1-3
+20% CR/LWAL+CDH/HBET:4-6
+8% CR/LWAL+CDH/HBET:7-</t>
+  </si>
+  <si>
+    <t>30% CR/LFINF+CDL/HBET:1-3
+45% CR/LFINF+CDL/HBET:4-6
+15% CR/LFINF+CDL/HBET:7-
+10% CR/LFINF+CDN/HBET:1-3</t>
+  </si>
+  <si>
+    <t>16% CR/LFINF(CL)+CDL/HBET:1-3
+44% CR/LFINF(CL)+CDL/HBET:4-6
+10% CR/LFINF(CL)+CDL/HBET:7-
+30% MUR+CL/LWAL+CDN/HBET:1-3</t>
+  </si>
+  <si>
+    <t>23% CR/LFINF(CL)+CDL/HBET:1-3
+44% CR/LFINF(CL)+CDL/HBET:4-6
+10% CR/LFINF(CL)+CDL/HBET:7-
+23% MUR+CL/LWAL+CDN/HBET:1-3</t>
+  </si>
+  <si>
+    <t>80% W/LFM+CDN/HBET:1-3
+20% W/LFM+CDL/HBET:1-3</t>
+  </si>
+  <si>
+    <t>35% CR/LWAL+CDL/HBET:1-3
+10% CR/LWAL+CDL/HBET:4-6
+55% MUR+CL/LWAL+CDN/HBET:1-3</t>
+  </si>
+  <si>
+    <t>45% CR/LWAL+CDL/HBET:1-3
+10% CR/LWAL+CDL/HBET:4-6
+45% MUR+CL/LWAL+CDN/HBET:1-3</t>
+  </si>
+  <si>
+    <t>80% W/LWAL+CDN/HBET:1-3
+20% W/LWAL+CDL/HBET:1-3</t>
+  </si>
+  <si>
+    <t>20% CR/LDUAL+CDH/HBET:1-3
+20% CR/LDUAL+CDH/HBET:4-6
 7% CR/LDUAL+CDH/HBET:7-
 25% CR/LWAL+CDH/HBET:1-3
 20% CR/LWAL+CDH/HBET:4-6
@@ -714,7 +672,7 @@
   <sheetData>
     <row r="1" spans="1:100" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -750,7 +708,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>11</v>
@@ -762,60 +720,60 @@
         <v>13</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="Q2" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -903,55 +861,55 @@
     </row>
     <row r="3" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="K3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="N3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="P3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -1039,55 +997,55 @@
     </row>
     <row r="4" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="L4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="O4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1210,7 +1168,7 @@
   <sheetData>
     <row r="1" spans="1:100" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1246,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>11</v>
@@ -1258,60 +1216,60 @@
         <v>13</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="Q2" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -1399,55 +1357,55 @@
     </row>
     <row r="3" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="K3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="N3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="P3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -1535,55 +1493,55 @@
     </row>
     <row r="4" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="L4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="O4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1678,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1706,7 +1664,7 @@
   <sheetData>
     <row r="1" spans="1:100" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1742,7 +1700,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>11</v>
@@ -1754,60 +1712,60 @@
         <v>13</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -1895,55 +1853,55 @@
     </row>
     <row r="3" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -2031,55 +1989,55 @@
     </row>
     <row r="4" spans="1:100" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>

</xml_diff>